<commit_message>
Corrige o nome da solução para "System Settings"
</commit_message>
<xml_diff>
--- a/others/customize.dashboard.dash/instances/2.dashboard-others_v6.35.0.xlsx
+++ b/others/customize.dashboard.dash/instances/2.dashboard-others_v6.35.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miguelmesquita/.local/share/cob-cli/customize.dashboard.dash/others/customize.dashboard.dash/instances/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hugomarcelino/projects/cob/client-solutions/server_afrigotel/others/customize.dashboard.dash/instances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70B66A0-A3EC-2046-BD69-4FCC239CDD23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4499E8-3259-B144-B8F8-FAE5CEF843D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12160" yWindow="6440" windowWidth="33460" windowHeight="17820" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12160" yWindow="6440" windowWidth="33460" windowHeight="17820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="&gt;InputVarKibana" sheetId="8" r:id="rId6"/>
     <sheet name="CONFIG" sheetId="14" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,6 +30,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -91,9 +92,6 @@
     <t>Width</t>
   </si>
   <si>
-    <t>Gestão CoB</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -535,6 +533,9 @@
   </si>
   <si>
     <t>Solutions Def Id</t>
+  </si>
+  <si>
+    <t>System Settings</t>
   </si>
 </sst>
 </file>
@@ -665,9 +666,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -705,7 +706,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -811,7 +812,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -953,7 +954,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -963,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1046,31 +1047,31 @@
         <v>-3</v>
       </c>
       <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
         <v>30</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" t="s">
         <v>31</v>
       </c>
-      <c r="G2" t="s">
-        <v>150</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" t="s">
         <v>32</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -1078,52 +1079,52 @@
         <v>-4</v>
       </c>
       <c r="B3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
       <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
         <v>34</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H3" t="s">
         <v>35</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>151</v>
-      </c>
-      <c r="H3" t="s">
-        <v>36</v>
-      </c>
       <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
         <v>21</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>22</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>23</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>24</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>25</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>26</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>27</v>
       </c>
-      <c r="P3" t="s">
-        <v>28</v>
-      </c>
       <c r="Q3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -1131,49 +1132,49 @@
         <v>-5</v>
       </c>
       <c r="B4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s">
         <v>21</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>22</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>23</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>24</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>25</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>26</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>27</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>28</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1198,13 +1199,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1215,7 +1216,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1226,7 +1227,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1237,7 +1238,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1271,40 +1272,40 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -1318,16 +1319,16 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" t="s">
         <v>59</v>
       </c>
-      <c r="G2" t="s">
-        <v>60</v>
-      </c>
       <c r="H2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -1341,7 +1342,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1355,16 +1356,16 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" t="s">
         <v>61</v>
       </c>
-      <c r="G4" t="s">
-        <v>62</v>
-      </c>
       <c r="H4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -1378,7 +1379,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1392,17 +1393,17 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F6" s="8" t="str">
         <f>CONFIG!B1</f>
         <v>SERVER NAME</v>
       </c>
       <c r="G6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -1416,7 +1417,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -1430,10 +1431,10 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -1447,13 +1448,13 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K9" t="s">
         <v>65</v>
       </c>
-      <c r="K9" t="s">
-        <v>66</v>
-      </c>
       <c r="L9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -1467,16 +1468,16 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -1490,7 +1491,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1504,10 +1505,10 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="I12" t="s">
         <v>52</v>
-      </c>
-      <c r="I12" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1521,13 +1522,13 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" t="s">
         <v>54</v>
       </c>
-      <c r="E13" t="s">
+      <c r="J13" t="s">
         <v>55</v>
-      </c>
-      <c r="J13" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1554,19 +1555,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1577,13 +1578,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" t="s">
         <v>74</v>
       </c>
-      <c r="D2" t="s">
-        <v>75</v>
-      </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1594,13 +1595,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" t="s">
         <v>76</v>
       </c>
-      <c r="D3" t="s">
-        <v>77</v>
-      </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1611,13 +1612,13 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" t="s">
         <v>78</v>
       </c>
-      <c r="D4" t="s">
-        <v>79</v>
-      </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1628,13 +1629,13 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" t="s">
         <v>80</v>
       </c>
-      <c r="D5" t="s">
-        <v>81</v>
-      </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1645,13 +1646,13 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1662,13 +1663,13 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1679,13 +1680,13 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1696,13 +1697,13 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1713,13 +1714,13 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" t="s">
         <v>71</v>
       </c>
-      <c r="D10" t="s">
-        <v>72</v>
-      </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1751,34 +1752,34 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1795,19 +1796,19 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" t="s">
         <v>97</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>98</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>99</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>100</v>
-      </c>
-      <c r="J2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -1824,19 +1825,19 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" t="s">
         <v>102</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>103</v>
       </c>
-      <c r="G3" t="s">
-        <v>104</v>
-      </c>
       <c r="I3" t="s">
+        <v>99</v>
+      </c>
+      <c r="J3" t="s">
         <v>100</v>
-      </c>
-      <c r="J3" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1853,20 +1854,20 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" t="s">
         <v>105</v>
-      </c>
-      <c r="F4" t="s">
-        <v>106</v>
       </c>
       <c r="G4" s="7" t="str">
         <f>"#/definitions/"&amp;CONFIG!B2&amp;"/q={{arg}}"</f>
         <v>#/definitions/1/q={{arg}}</v>
       </c>
       <c r="I4" t="s">
+        <v>99</v>
+      </c>
+      <c r="J4" t="s">
         <v>100</v>
-      </c>
-      <c r="J4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -1883,19 +1884,19 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" t="s">
         <v>107</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>108</v>
       </c>
-      <c r="G5" t="s">
-        <v>109</v>
-      </c>
       <c r="I5" t="s">
+        <v>99</v>
+      </c>
+      <c r="J5" t="s">
         <v>100</v>
-      </c>
-      <c r="J5" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -1912,19 +1913,19 @@
         <v>4</v>
       </c>
       <c r="E6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" t="s">
         <v>110</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>111</v>
       </c>
-      <c r="G6" t="s">
-        <v>112</v>
-      </c>
       <c r="I6" t="s">
+        <v>99</v>
+      </c>
+      <c r="J6" t="s">
         <v>100</v>
-      </c>
-      <c r="J6" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -1941,16 +1942,16 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G7" t="s">
         <v>113</v>
       </c>
-      <c r="G7" t="s">
-        <v>114</v>
-      </c>
       <c r="I7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -1967,19 +1968,19 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" t="s">
         <v>102</v>
       </c>
-      <c r="F8" t="s">
-        <v>103</v>
-      </c>
       <c r="G8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I8" t="s">
+        <v>99</v>
+      </c>
+      <c r="J8" t="s">
         <v>100</v>
-      </c>
-      <c r="J8" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -1996,19 +1997,19 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F9" t="s">
         <v>116</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>117</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>118</v>
       </c>
-      <c r="I9" t="s">
-        <v>119</v>
-      </c>
       <c r="J9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -2025,19 +2026,19 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
+        <v>119</v>
+      </c>
+      <c r="F10" t="s">
+        <v>107</v>
+      </c>
+      <c r="G10" t="s">
         <v>120</v>
       </c>
-      <c r="F10" t="s">
-        <v>108</v>
-      </c>
-      <c r="G10" t="s">
-        <v>121</v>
-      </c>
       <c r="I10" t="s">
+        <v>99</v>
+      </c>
+      <c r="J10" t="s">
         <v>100</v>
-      </c>
-      <c r="J10" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -2054,19 +2055,19 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
+        <v>121</v>
+      </c>
+      <c r="F11" t="s">
+        <v>116</v>
+      </c>
+      <c r="G11" t="s">
         <v>122</v>
       </c>
-      <c r="F11" t="s">
-        <v>117</v>
-      </c>
-      <c r="G11" t="s">
-        <v>123</v>
-      </c>
       <c r="I11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -2083,20 +2084,20 @@
         <v>4</v>
       </c>
       <c r="E12" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" t="s">
         <v>105</v>
-      </c>
-      <c r="F12" t="s">
-        <v>106</v>
       </c>
       <c r="G12" s="7" t="str">
         <f>"#/definitions/"&amp;CONFIG!B2&amp;"/q={{arg}}"</f>
         <v>#/definitions/1/q={{arg}}</v>
       </c>
       <c r="I12" t="s">
+        <v>99</v>
+      </c>
+      <c r="J12" t="s">
         <v>100</v>
-      </c>
-      <c r="J12" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -2113,19 +2114,19 @@
         <v>5</v>
       </c>
       <c r="E13" t="s">
+        <v>123</v>
+      </c>
+      <c r="F13" t="s">
+        <v>116</v>
+      </c>
+      <c r="G13" t="s">
         <v>124</v>
       </c>
-      <c r="F13" t="s">
-        <v>117</v>
-      </c>
-      <c r="G13" t="s">
-        <v>125</v>
-      </c>
       <c r="I13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -2142,20 +2143,20 @@
         <v>6</v>
       </c>
       <c r="E14" t="s">
+        <v>125</v>
+      </c>
+      <c r="F14" t="s">
         <v>126</v>
-      </c>
-      <c r="F14" t="s">
-        <v>127</v>
       </c>
       <c r="G14" s="7" t="str">
         <f>"#/definitions/"&amp;CONFIG!B3&amp;"/q="</f>
         <v>#/definitions/2/q=</v>
       </c>
       <c r="I14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -2172,20 +2173,20 @@
         <v>7</v>
       </c>
       <c r="E15" t="s">
+        <v>128</v>
+      </c>
+      <c r="F15" t="s">
         <v>129</v>
-      </c>
-      <c r="F15" t="s">
-        <v>130</v>
       </c>
       <c r="G15" s="7" t="str">
         <f>"#/definitions/"&amp;CONFIG!B4&amp;"/q="</f>
         <v>#/definitions/3/q=</v>
       </c>
       <c r="I15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -2202,20 +2203,20 @@
         <v>8</v>
       </c>
       <c r="E16" t="s">
+        <v>131</v>
+      </c>
+      <c r="F16" t="s">
         <v>132</v>
-      </c>
-      <c r="F16" t="s">
-        <v>133</v>
       </c>
       <c r="G16" s="7" t="str">
         <f>"#/definitions/"&amp;CONFIG!B5&amp;"/q="</f>
         <v>#/definitions/4/q=</v>
       </c>
       <c r="I16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -2232,19 +2233,19 @@
         <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F17" t="s">
+        <v>134</v>
+      </c>
+      <c r="G17" t="s">
         <v>135</v>
       </c>
-      <c r="G17" t="s">
-        <v>136</v>
-      </c>
       <c r="I17" t="s">
+        <v>99</v>
+      </c>
+      <c r="J17" t="s">
         <v>100</v>
-      </c>
-      <c r="J17" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -2261,19 +2262,19 @@
         <v>10</v>
       </c>
       <c r="E18" t="s">
+        <v>136</v>
+      </c>
+      <c r="F18" t="s">
+        <v>116</v>
+      </c>
+      <c r="G18" t="s">
         <v>137</v>
       </c>
-      <c r="F18" t="s">
-        <v>117</v>
-      </c>
-      <c r="G18" t="s">
-        <v>138</v>
-      </c>
       <c r="I18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -2290,19 +2291,19 @@
         <v>11</v>
       </c>
       <c r="E19" t="s">
+        <v>138</v>
+      </c>
+      <c r="F19" t="s">
         <v>139</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>140</v>
       </c>
-      <c r="G19" t="s">
-        <v>141</v>
-      </c>
       <c r="I19" t="s">
+        <v>99</v>
+      </c>
+      <c r="J19" t="s">
         <v>100</v>
-      </c>
-      <c r="J19" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -2319,19 +2320,19 @@
         <v>12</v>
       </c>
       <c r="E20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F20" t="s">
+        <v>116</v>
+      </c>
+      <c r="G20" t="s">
         <v>142</v>
       </c>
-      <c r="F20" t="s">
-        <v>117</v>
-      </c>
-      <c r="G20" t="s">
-        <v>143</v>
-      </c>
       <c r="I20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -2348,19 +2349,19 @@
         <v>13</v>
       </c>
       <c r="E21" t="s">
+        <v>143</v>
+      </c>
+      <c r="F21" t="s">
         <v>144</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>145</v>
       </c>
-      <c r="G21" t="s">
-        <v>146</v>
-      </c>
       <c r="I21" t="s">
+        <v>99</v>
+      </c>
+      <c r="J21" t="s">
         <v>100</v>
-      </c>
-      <c r="J21" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -2377,19 +2378,19 @@
         <v>0</v>
       </c>
       <c r="E22" t="s">
+        <v>146</v>
+      </c>
+      <c r="F22" t="s">
         <v>147</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>148</v>
       </c>
-      <c r="G22" t="s">
-        <v>149</v>
-      </c>
       <c r="I22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2414,19 +2415,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
-        <v>42</v>
-      </c>
       <c r="D1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" t="s">
         <v>87</v>
-      </c>
-      <c r="E1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2443,7 +2444,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2458,8 +2459,8 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2471,15 +2472,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
@@ -2487,7 +2488,7 @@
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B3" s="5">
         <v>2</v>
@@ -2495,7 +2496,7 @@
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B4" s="5">
         <v>3</v>
@@ -2503,7 +2504,7 @@
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B5" s="5">
         <v>4</v>

</xml_diff>